<commit_message>
<55 year old female splines
</commit_message>
<xml_diff>
--- a/data/l55_Female_first_revision.xlsx
+++ b/data/l55_Female_first_revision.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="234" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB6B13B1-8800-45EC-8B41-9ED86E8D1DB5}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rcs_first_revision_mean" sheetId="1" r:id="rId1"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1846,7 +1846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E49F2D1-14B2-4EC2-9544-01485EF4F928}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>

</xml_diff>